<commit_message>
Finished the data convertion process
Added the datasets to the main folder and added two column that contain the data in the correct units (c=1, km and solar mass)
</commit_message>
<xml_diff>
--- a/middle.xlsx
+++ b/middle.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15149eb1c9cf386c/Escritorio/TFG/Codigo-GIT/TFG/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_D0521FC397D9AECF8A160B6B037745C85BB6731B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E482836B-14B6-4FF1-8B54-760B3E51FE24}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
   <si>
     <t>x</t>
   </si>
@@ -22,9 +41,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>0.0157273918741808</t>
-  </si>
-  <si>
     <t>0.0346002621231979</t>
   </si>
   <si>
@@ -401,13 +417,19 @@
   </si>
   <si>
     <t>3.972461273666090</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Pressure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,13 +492,25 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -514,7 +548,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -548,6 +582,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -582,9 +617,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -757,555 +793,1099 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1.5727391874180801E-2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <f>A2/1.4765679173556</f>
+        <v>1.0651316264779167E-2</v>
+      </c>
+      <c r="D2">
+        <f>B2/1.4765679173556</f>
+        <v>4.6626243889997315E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:D66" si="0">A3/1.4765679173556</f>
+        <v>2.343289578251426E-2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>4.6626243889997315E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>3.7279606926727216E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>9.3252487779994491E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5.2191449697418103E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>9.3252487779994491E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>6.816842409458658E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1.398787316699914E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>8.3080266865277336E-2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.398787316699914E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>9.6926978009490211E-2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.398787316699914E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.1107736891537031</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.398787316699914E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.12568553192439455</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.398787316699914E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.14485790120099673</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.3313121944998655E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.15976974397168747</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2.3313121944998655E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.18000724487476824</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3.7300995111997866E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.19172369276602538</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>5.5951492667996761E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.20557040391023826</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>7.4601990223995593E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.21728685180149543</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>8.3927239001994697E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.2321986945721862</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.1072403609469935</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.2428500108369655</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.13055348289199228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.25882698523413411</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0.1631918536149902</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.27054343312539125</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0.19116759994898888</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0.28012961776369272</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.22846859506098666</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.29397632890790559</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0.26110696578398457</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.30782304005211847</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.30773320967398221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0.31634409306394207</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.34037158039698007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0.33019080420815494</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0.38699782428697765</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0.33871185721997854</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0.43362406817697524</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0.34616777860532422</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0.48491293645597205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0.35681909487010288</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0.5222139315679698</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0.36640527950840429</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0.57350279984696728</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>0.3759914641467057</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0.63411691690396388</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0.3845125171585293</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0.68540578518295803</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>0.3940987017968301</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0.73669465346195206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0.40048949155569796</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>0.78332089735195098</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>0.41007567619399937</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>0.82994714124195001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>0.41753159757934444</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>0.89522388268794306</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>0.42605265059116793</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>0.95117537535593921</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>0.43137830872355798</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>0.99780161924593802</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>0.44096449336185878</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>1.0537531119139341</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>0.44842041474720445</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>1.1097046045819301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>0.456941467759028</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>1.1656560972499328</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>0.46439738914437312</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>1.2169449655289271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>0.47185331052971879</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>1.263571209418926</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>0.4814394951680202</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>1.31486007769792</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>0.48996054817984308</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>1.3708115703659161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>0.49848160119166668</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>1.422100438644917</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>0.50593752257701241</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>1.473389306923911</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>0.51552370721531315</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>1.5386660483699108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>0.52297962860065894</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>1.5946175410379069</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>0.53043554998600462</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>1.6552316580949049</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>0.53895660299782744</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>1.6971952775959018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>0.54641252438317323</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>1.7578093946528999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>0.55280331414204043</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>1.8137608873208959</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>0.55919410390090829</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>1.8603871312108879</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>0.56665002528625397</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>1.9116759994898889</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>0.57304081504512117</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>1.9676274921578847</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>55</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>0.58156186805694476</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>2.0189163604368789</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>0.58795265781581185</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>2.079530477493877</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>0.59540857920115753</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>2.1401445945508746</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>0.60499476383945905</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>2.1914334628298691</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>0.61245068522480406</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>2.2473849554978718</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>0.617776343357194</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>2.3173243213328667</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>0.6241671331160612</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>2.3639505652228587</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>0.63055792287492907</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>2.4199020578908619</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>0.63694871263379627</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>2.4711909261698559</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>0.64653489727209768</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>2.5318050432268535</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>0.65292568703096487</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>2.5924191602838516</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
+      <c r="C67">
+        <f t="shared" ref="C67:D68" si="1">A67/1.4765679173556</f>
+        <v>0.65825134516335482</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="1"/>
+        <v>2.6483706529518476</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>67</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" t="s">
-        <v>128</v>
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>0.66464213492222268</v>
+      </c>
+      <c r="D68">
+        <f>B68/1.4765679173556</f>
+        <v>2.6903342724528447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the units again
Forgot that the data is normalized to different units of 10
</commit_message>
<xml_diff>
--- a/middle.xlsx
+++ b/middle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15149eb1c9cf386c/Escritorio/TFG/Codigo-GIT/TFG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_D0521FC397D9AECF8A160B6B037745C85BB6731B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E482836B-14B6-4FF1-8B54-760B3E51FE24}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_D0521FC397D9AECF8A160B6B037745C85BB6731B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1EF909A-E30F-4B63-BB71-2FF558038016}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -797,10 +797,13 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="D2" sqref="D2:D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -824,12 +827,12 @@
         <v>68</v>
       </c>
       <c r="C2">
-        <f>A2/1.4765679173556</f>
-        <v>1.0651316264779167E-2</v>
+        <f>A2/1.4765679173556 * 10^(-3)</f>
+        <v>1.0651316264779167E-5</v>
       </c>
       <c r="D2">
-        <f>B2/1.4765679173556</f>
-        <v>4.6626243889997315E-3</v>
+        <f>B2/1.4765679173556 * 10^(-4)</f>
+        <v>4.6626243889997319E-7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -840,12 +843,12 @@
         <v>68</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:D66" si="0">A3/1.4765679173556</f>
-        <v>2.343289578251426E-2</v>
+        <f t="shared" ref="C3:C66" si="0">A3/1.4765679173556 * 10^(-3)</f>
+        <v>2.3432895782514262E-5</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
-        <v>4.6626243889997315E-3</v>
+        <f t="shared" ref="D3:D66" si="1">B3/1.4765679173556 * 10^(-4)</f>
+        <v>4.6626243889997319E-7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -857,11 +860,11 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>3.7279606926727216E-2</v>
+        <v>3.7279606926727219E-5</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>9.3252487779994491E-3</v>
+        <f t="shared" si="1"/>
+        <v>9.3252487779994501E-7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -873,11 +876,11 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>5.2191449697418103E-2</v>
+        <v>5.2191449697418106E-5</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>9.3252487779994491E-3</v>
+        <f t="shared" si="1"/>
+        <v>9.3252487779994501E-7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -889,11 +892,11 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>6.816842409458658E-2</v>
+        <v>6.8168424094586585E-5</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>1.398787316699914E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.3987873166999141E-6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -905,11 +908,11 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>8.3080266865277336E-2</v>
+        <v>8.3080266865277337E-5</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>1.398787316699914E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.3987873166999141E-6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -921,11 +924,11 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>9.6926978009490211E-2</v>
+        <v>9.6926978009490207E-5</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.398787316699914E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.3987873166999141E-6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -937,11 +940,11 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0.1107736891537031</v>
+        <v>1.107736891537031E-4</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>1.398787316699914E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.3987873166999141E-6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -953,11 +956,11 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.12568553192439455</v>
+        <v>1.2568553192439456E-4</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1.398787316699914E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.3987873166999141E-6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -969,11 +972,11 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.14485790120099673</v>
+        <v>1.4485790120099672E-4</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>2.3313121944998655E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.3313121944998655E-6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -985,11 +988,11 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0.15976974397168747</v>
+        <v>1.5976974397168749E-4</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>2.3313121944998655E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.3313121944998655E-6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1001,11 +1004,11 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0.18000724487476824</v>
+        <v>1.8000724487476824E-4</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>3.7300995111997866E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.7300995111997868E-6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1017,11 +1020,11 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0.19172369276602538</v>
+        <v>1.9172369276602538E-4</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>5.5951492667996761E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.595149266799676E-6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1033,11 +1036,11 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.20557040391023826</v>
+        <v>2.0557040391023826E-4</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>7.4601990223995593E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.4601990223995601E-6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1049,11 +1052,11 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.21728685180149543</v>
+        <v>2.1728685180149543E-4</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>8.3927239001994697E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.3927239001994703E-6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1065,11 +1068,11 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.2321986945721862</v>
+        <v>2.321986945721862E-4</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0.1072403609469935</v>
+        <f t="shared" si="1"/>
+        <v>1.072403609469935E-5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1081,11 +1084,11 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.2428500108369655</v>
+        <v>2.4285001083696551E-4</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0.13055348289199228</v>
+        <f t="shared" si="1"/>
+        <v>1.3055348289199228E-5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1097,11 +1100,11 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.25882698523413411</v>
+        <v>2.5882698523413411E-4</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>0.1631918536149902</v>
+        <f t="shared" si="1"/>
+        <v>1.6319185361499022E-5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1113,11 +1116,11 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>0.27054343312539125</v>
+        <v>2.7054343312539128E-4</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>0.19116759994898888</v>
+        <f t="shared" si="1"/>
+        <v>1.911675999489889E-5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1129,11 +1132,11 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>0.28012961776369272</v>
+        <v>2.8012961776369274E-4</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0.22846859506098666</v>
+        <f t="shared" si="1"/>
+        <v>2.2846859506098667E-5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1145,11 +1148,11 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>0.29397632890790559</v>
+        <v>2.9397632890790562E-4</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0.26110696578398457</v>
+        <f t="shared" si="1"/>
+        <v>2.6110696578398457E-5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1161,11 +1164,11 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>0.30782304005211847</v>
+        <v>3.0782304005211845E-4</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
-        <v>0.30773320967398221</v>
+        <f t="shared" si="1"/>
+        <v>3.077332096739822E-5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1177,11 +1180,11 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>0.31634409306394207</v>
+        <v>3.1634409306394206E-4</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
-        <v>0.34037158039698007</v>
+        <f t="shared" si="1"/>
+        <v>3.4037158039698007E-5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1193,11 +1196,11 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>0.33019080420815494</v>
+        <v>3.3019080420815494E-4</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
-        <v>0.38699782428697765</v>
+        <f t="shared" si="1"/>
+        <v>3.869978242869777E-5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1209,11 +1212,11 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>0.33871185721997854</v>
+        <v>3.3871185721997854E-4</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
-        <v>0.43362406817697524</v>
+        <f t="shared" si="1"/>
+        <v>4.3362406817697526E-5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1225,11 +1228,11 @@
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>0.34616777860532422</v>
+        <v>3.4616777860532424E-4</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
-        <v>0.48491293645597205</v>
+        <f t="shared" si="1"/>
+        <v>4.8491293645597205E-5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1241,11 +1244,11 @@
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>0.35681909487010288</v>
+        <v>3.568190948701029E-4</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
-        <v>0.5222139315679698</v>
+        <f t="shared" si="1"/>
+        <v>5.2221393156796981E-5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1257,11 +1260,11 @@
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>0.36640527950840429</v>
+        <v>3.6640527950840431E-4</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
-        <v>0.57350279984696728</v>
+        <f t="shared" si="1"/>
+        <v>5.7350279984696728E-5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1273,11 +1276,11 @@
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>0.3759914641467057</v>
+        <v>3.7599146414670571E-4</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
-        <v>0.63411691690396388</v>
+        <f t="shared" si="1"/>
+        <v>6.3411691690396386E-5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1289,11 +1292,11 @@
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>0.3845125171585293</v>
+        <v>3.8451251715852932E-4</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
-        <v>0.68540578518295803</v>
+        <f t="shared" si="1"/>
+        <v>6.85405785182958E-5</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1305,11 +1308,11 @@
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>0.3940987017968301</v>
+        <v>3.9409870179683013E-4</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
-        <v>0.73669465346195206</v>
+        <f t="shared" si="1"/>
+        <v>7.3669465346195214E-5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1321,11 +1324,11 @@
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>0.40048949155569796</v>
+        <v>4.0048949155569797E-4</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
-        <v>0.78332089735195098</v>
+        <f t="shared" si="1"/>
+        <v>7.8332089735195099E-5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1337,11 +1340,11 @@
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>0.41007567619399937</v>
+        <v>4.1007567619399937E-4</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
-        <v>0.82994714124195001</v>
+        <f t="shared" si="1"/>
+        <v>8.2994714124195012E-5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1353,11 +1356,11 @@
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>0.41753159757934444</v>
+        <v>4.1753159757934447E-4</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
-        <v>0.89522388268794306</v>
+        <f t="shared" si="1"/>
+        <v>8.9522388268794314E-5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1369,11 +1372,11 @@
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>0.42605265059116793</v>
+        <v>4.2605265059116791E-4</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
-        <v>0.95117537535593921</v>
+        <f t="shared" si="1"/>
+        <v>9.5117537535593921E-5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1385,11 +1388,11 @@
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>0.43137830872355798</v>
+        <v>4.31378308723558E-4</v>
       </c>
       <c r="D37">
-        <f t="shared" si="0"/>
-        <v>0.99780161924593802</v>
+        <f t="shared" si="1"/>
+        <v>9.9780161924593807E-5</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1401,11 +1404,11 @@
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>0.44096449336185878</v>
+        <v>4.4096449336185876E-4</v>
       </c>
       <c r="D38">
-        <f t="shared" si="0"/>
-        <v>1.0537531119139341</v>
+        <f t="shared" si="1"/>
+        <v>1.0537531119139341E-4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1417,11 +1420,11 @@
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>0.44842041474720445</v>
+        <v>4.4842041474720445E-4</v>
       </c>
       <c r="D39">
-        <f t="shared" si="0"/>
-        <v>1.1097046045819301</v>
+        <f t="shared" si="1"/>
+        <v>1.1097046045819302E-4</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1433,11 +1436,11 @@
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>0.456941467759028</v>
+        <v>4.56941467759028E-4</v>
       </c>
       <c r="D40">
-        <f t="shared" si="0"/>
-        <v>1.1656560972499328</v>
+        <f t="shared" si="1"/>
+        <v>1.1656560972499328E-4</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1449,11 +1452,11 @@
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>0.46439738914437312</v>
+        <v>4.643973891443731E-4</v>
       </c>
       <c r="D41">
-        <f t="shared" si="0"/>
-        <v>1.2169449655289271</v>
+        <f t="shared" si="1"/>
+        <v>1.2169449655289271E-4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1465,11 +1468,11 @@
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>0.47185331052971879</v>
+        <v>4.718533105297188E-4</v>
       </c>
       <c r="D42">
-        <f t="shared" si="0"/>
-        <v>1.263571209418926</v>
+        <f t="shared" si="1"/>
+        <v>1.2635712094189261E-4</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1481,11 +1484,11 @@
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>0.4814394951680202</v>
+        <v>4.814394951680202E-4</v>
       </c>
       <c r="D43">
-        <f t="shared" si="0"/>
-        <v>1.31486007769792</v>
+        <f t="shared" si="1"/>
+        <v>1.3148600776979202E-4</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1497,11 +1500,11 @@
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>0.48996054817984308</v>
+        <v>4.899605481798431E-4</v>
       </c>
       <c r="D44">
-        <f t="shared" si="0"/>
-        <v>1.3708115703659161</v>
+        <f t="shared" si="1"/>
+        <v>1.370811570365916E-4</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1513,11 +1516,11 @@
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>0.49848160119166668</v>
+        <v>4.9848160119166671E-4</v>
       </c>
       <c r="D45">
-        <f t="shared" si="0"/>
-        <v>1.422100438644917</v>
+        <f t="shared" si="1"/>
+        <v>1.4221004386449169E-4</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1529,11 +1532,11 @@
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>0.50593752257701241</v>
+        <v>5.059375225770124E-4</v>
       </c>
       <c r="D46">
-        <f t="shared" si="0"/>
-        <v>1.473389306923911</v>
+        <f t="shared" si="1"/>
+        <v>1.4733893069239111E-4</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1545,11 +1548,11 @@
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>0.51552370721531315</v>
+        <v>5.1552370721531316E-4</v>
       </c>
       <c r="D47">
-        <f t="shared" si="0"/>
-        <v>1.5386660483699108</v>
+        <f t="shared" si="1"/>
+        <v>1.538666048369911E-4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1561,11 +1564,11 @@
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>0.52297962860065894</v>
+        <v>5.2297962860065896E-4</v>
       </c>
       <c r="D48">
-        <f t="shared" si="0"/>
-        <v>1.5946175410379069</v>
+        <f t="shared" si="1"/>
+        <v>1.5946175410379071E-4</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1577,11 +1580,11 @@
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>0.53043554998600462</v>
+        <v>5.3043554998600465E-4</v>
       </c>
       <c r="D49">
-        <f t="shared" si="0"/>
-        <v>1.6552316580949049</v>
+        <f t="shared" si="1"/>
+        <v>1.6552316580949051E-4</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1593,11 +1596,11 @@
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>0.53895660299782744</v>
+        <v>5.389566029978275E-4</v>
       </c>
       <c r="D50">
-        <f t="shared" si="0"/>
-        <v>1.6971952775959018</v>
+        <f t="shared" si="1"/>
+        <v>1.6971952775959019E-4</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1609,11 +1612,11 @@
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>0.54641252438317323</v>
+        <v>5.4641252438317319E-4</v>
       </c>
       <c r="D51">
-        <f t="shared" si="0"/>
-        <v>1.7578093946528999</v>
+        <f t="shared" si="1"/>
+        <v>1.7578093946528999E-4</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1625,11 +1628,11 @@
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>0.55280331414204043</v>
+        <v>5.5280331414204044E-4</v>
       </c>
       <c r="D52">
-        <f t="shared" si="0"/>
-        <v>1.8137608873208959</v>
+        <f t="shared" si="1"/>
+        <v>1.8137608873208959E-4</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1641,11 +1644,11 @@
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>0.55919410390090829</v>
+        <v>5.5919410390090833E-4</v>
       </c>
       <c r="D53">
-        <f t="shared" si="0"/>
-        <v>1.8603871312108879</v>
+        <f t="shared" si="1"/>
+        <v>1.8603871312108882E-4</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1657,11 +1660,11 @@
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>0.56665002528625397</v>
+        <v>5.6665002528625402E-4</v>
       </c>
       <c r="D54">
-        <f t="shared" si="0"/>
-        <v>1.9116759994898889</v>
+        <f t="shared" si="1"/>
+        <v>1.9116759994898891E-4</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1673,11 +1676,11 @@
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>0.57304081504512117</v>
+        <v>5.7304081504512116E-4</v>
       </c>
       <c r="D55">
-        <f t="shared" si="0"/>
-        <v>1.9676274921578847</v>
+        <f t="shared" si="1"/>
+        <v>1.9676274921578849E-4</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1689,11 +1692,11 @@
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>0.58156186805694476</v>
+        <v>5.8156186805694476E-4</v>
       </c>
       <c r="D56">
-        <f t="shared" si="0"/>
-        <v>2.0189163604368789</v>
+        <f t="shared" si="1"/>
+        <v>2.018916360436879E-4</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1705,11 +1708,11 @@
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
-        <v>0.58795265781581185</v>
+        <v>5.879526578158119E-4</v>
       </c>
       <c r="D57">
-        <f t="shared" si="0"/>
-        <v>2.079530477493877</v>
+        <f t="shared" si="1"/>
+        <v>2.079530477493877E-4</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1721,11 +1724,11 @@
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>0.59540857920115753</v>
+        <v>5.9540857920115759E-4</v>
       </c>
       <c r="D58">
-        <f t="shared" si="0"/>
-        <v>2.1401445945508746</v>
+        <f t="shared" si="1"/>
+        <v>2.1401445945508748E-4</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1737,11 +1740,11 @@
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>0.60499476383945905</v>
+        <v>6.0499476383945911E-4</v>
       </c>
       <c r="D59">
-        <f t="shared" si="0"/>
-        <v>2.1914334628298691</v>
+        <f t="shared" si="1"/>
+        <v>2.1914334628298692E-4</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1753,11 +1756,11 @@
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>0.61245068522480406</v>
+        <v>6.1245068522480404E-4</v>
       </c>
       <c r="D60">
-        <f t="shared" si="0"/>
-        <v>2.2473849554978718</v>
+        <f t="shared" si="1"/>
+        <v>2.2473849554978717E-4</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1769,11 +1772,11 @@
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>0.617776343357194</v>
+        <v>6.1777634335719402E-4</v>
       </c>
       <c r="D61">
-        <f t="shared" si="0"/>
-        <v>2.3173243213328667</v>
+        <f t="shared" si="1"/>
+        <v>2.3173243213328668E-4</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1785,11 +1788,11 @@
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>0.6241671331160612</v>
+        <v>6.2416713311606127E-4</v>
       </c>
       <c r="D62">
-        <f t="shared" si="0"/>
-        <v>2.3639505652228587</v>
+        <f t="shared" si="1"/>
+        <v>2.3639505652228588E-4</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1801,11 +1804,11 @@
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
-        <v>0.63055792287492907</v>
+        <v>6.3055792287492905E-4</v>
       </c>
       <c r="D63">
-        <f t="shared" si="0"/>
-        <v>2.4199020578908619</v>
+        <f t="shared" si="1"/>
+        <v>2.4199020578908619E-4</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1817,11 +1820,11 @@
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
-        <v>0.63694871263379627</v>
+        <v>6.3694871263379629E-4</v>
       </c>
       <c r="D64">
-        <f t="shared" si="0"/>
-        <v>2.4711909261698559</v>
+        <f t="shared" si="1"/>
+        <v>2.471190926169856E-4</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1833,11 +1836,11 @@
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>0.64653489727209768</v>
+        <v>6.465348972720977E-4</v>
       </c>
       <c r="D65">
-        <f t="shared" si="0"/>
-        <v>2.5318050432268535</v>
+        <f t="shared" si="1"/>
+        <v>2.5318050432268538E-4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1849,11 +1852,11 @@
       </c>
       <c r="C66">
         <f t="shared" si="0"/>
-        <v>0.65292568703096487</v>
+        <v>6.5292568703096483E-4</v>
       </c>
       <c r="D66">
-        <f t="shared" si="0"/>
-        <v>2.5924191602838516</v>
+        <f t="shared" si="1"/>
+        <v>2.5924191602838515E-4</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1864,12 +1867,12 @@
         <v>126</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:D68" si="1">A67/1.4765679173556</f>
-        <v>0.65825134516335482</v>
+        <f t="shared" ref="C67:C68" si="2">A67/1.4765679173556 * 10^(-3)</f>
+        <v>6.5825134516335482E-4</v>
       </c>
       <c r="D67">
-        <f t="shared" si="1"/>
-        <v>2.6483706529518476</v>
+        <f t="shared" ref="D67:D68" si="3">B67/1.4765679173556 * 10^(-4)</f>
+        <v>2.6483706529518476E-4</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1880,12 +1883,12 @@
         <v>127</v>
       </c>
       <c r="C68">
-        <f t="shared" si="1"/>
-        <v>0.66464213492222268</v>
+        <f t="shared" si="2"/>
+        <v>6.6464213492222271E-4</v>
       </c>
       <c r="D68">
-        <f>B68/1.4765679173556</f>
-        <v>2.6903342724528447</v>
+        <f t="shared" si="3"/>
+        <v>2.6903342724528446E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>